<commit_message>
Uploaded runtime of some of the networks
</commit_message>
<xml_diff>
--- a/Structure tables report.xlsx
+++ b/Structure tables report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gines\Desktop\DLVR_3DReconstruction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEF307DC-86A3-4A06-9418-F0AC292A0319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F40C5F-8795-4462-9AB9-A8D501E7CEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{E12666EA-FB6F-4139-A86C-FF6F095F9F2F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12666EA-FB6F-4139-A86C-FF6F095F9F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Net</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>Paper</t>
+  </si>
+  <si>
+    <t>InceptionNet</t>
+  </si>
+  <si>
+    <t>Overlaps</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -432,131 +447,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574D92E5-B77D-4ABF-923C-B73F1B547486}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" t="s">
+      <c r="H1" s="1"/>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5">
+        <v>2.2389999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6">
+        <v>1.1870000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8">
+        <v>1.2390000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F11" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G11" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+  <mergeCells count="6">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Upload available data into report tables
</commit_message>
<xml_diff>
--- a/Structure tables report.xlsx
+++ b/Structure tables report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gines\Desktop\DLVR_3DReconstruction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F40C5F-8795-4462-9AB9-A8D501E7CEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F99AFC5-6478-48CB-9F6B-F02227866926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12666EA-FB6F-4139-A86C-FF6F095F9F2F}"/>
   </bookViews>
@@ -99,6 +99,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,11 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,35 +454,32 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" t="s">
+      <c r="I1" s="1"/>
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -486,24 +487,27 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -511,33 +515,84 @@
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1">
+        <f>231624+268281+268299</f>
+        <v>768204</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2.02</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
         <v>17</v>
+      </c>
+      <c r="J4">
+        <v>1.048</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1">
+        <v>1989452</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
+      <c r="D5">
+        <v>9.4419390000000006E-2</v>
+      </c>
+      <c r="E5">
+        <v>2.0852651999999998</v>
+      </c>
+      <c r="F5">
+        <v>5.2368394999999998E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.2609648</v>
+      </c>
+      <c r="H5">
+        <v>4.0598615999999997E-2</v>
+      </c>
       <c r="I5">
+        <v>0.95629405999999995</v>
+      </c>
+      <c r="J5">
         <v>2.2389999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
+      <c r="D6">
+        <v>9.0334860000000003E-2</v>
+      </c>
+      <c r="E6">
+        <v>2.2049370000000001</v>
+      </c>
+      <c r="F6">
+        <v>5.8732573000000003E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.6956241999999999</v>
+      </c>
+      <c r="H6">
+        <v>5.3862236000000001E-2</v>
+      </c>
       <c r="I6">
+        <v>1.6813327</v>
+      </c>
+      <c r="J6">
         <v>1.1870000000000001</v>
       </c>
     </row>
@@ -545,27 +600,52 @@
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1">
+        <v>10756132</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
+      </c>
+      <c r="J7">
+        <v>2.4060000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
         <v>17</v>
       </c>
+      <c r="D8">
+        <v>0.10224973</v>
+      </c>
+      <c r="E8">
+        <v>2.5022663999999999</v>
+      </c>
+      <c r="F8">
+        <v>8.1050046000000001E-2</v>
+      </c>
+      <c r="G8">
+        <v>1.6728656</v>
+      </c>
+      <c r="H8">
+        <v>6.6498085999999998E-2</v>
+      </c>
       <c r="I8">
+        <v>1.6730210000000001</v>
+      </c>
+      <c r="J8">
         <v>1.2390000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>12</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -573,22 +653,22 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>6</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>6</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>5</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -608,14 +688,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uploaded weights except for baseline
</commit_message>
<xml_diff>
--- a/Structure tables report.xlsx
+++ b/Structure tables report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gines\Desktop\DLVR_3DReconstruction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F99AFC5-6478-48CB-9F6B-F02227866926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294D50A1-7CCD-48A7-BD65-95B075A5E5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12666EA-FB6F-4139-A86C-FF6F095F9F2F}"/>
+    <workbookView xWindow="-17280" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{E12666EA-FB6F-4139-A86C-FF6F095F9F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,10 +133,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,18 +466,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="2"/>
       <c r="J1" t="s">
         <v>7</v>
       </c>
@@ -512,23 +512,23 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <f>231624+268281+268299</f>
         <v>768204</v>
       </c>
       <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>2.02</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>17</v>
       </c>
@@ -537,10 +537,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>1989452</v>
       </c>
       <c r="C5" t="s">
@@ -569,8 +569,8 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" t="s">
         <v>17</v>
       </c>
@@ -597,22 +597,40 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>10756132</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
+      <c r="D7">
+        <v>0.117326826</v>
+      </c>
+      <c r="E7">
+        <v>2.5623705000000001</v>
+      </c>
+      <c r="F7">
+        <v>9.1901064000000005E-2</v>
+      </c>
+      <c r="G7">
+        <v>1.9458221</v>
+      </c>
+      <c r="H7">
+        <v>7.9053940000000003E-2</v>
+      </c>
+      <c r="I7">
+        <v>1.6741633</v>
+      </c>
       <c r="J7">
         <v>2.4060000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Report table finished (categorical part remaining)
</commit_message>
<xml_diff>
--- a/Structure tables report.xlsx
+++ b/Structure tables report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gines\Desktop\DLVR_3DReconstruction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294D50A1-7CCD-48A7-BD65-95B075A5E5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4B1FB3-2BFE-45F3-992A-9E14E9F4B02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17280" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{E12666EA-FB6F-4139-A86C-FF6F095F9F2F}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12666EA-FB6F-4139-A86C-FF6F095F9F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>Net</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574D92E5-B77D-4ABF-923C-B73F1B547486}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,7 +468,7 @@
     <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
@@ -481,8 +484,11 @@
       <c r="J1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -511,7 +517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -522,21 +528,65 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
+      <c r="D3">
+        <v>0.13387018000000001</v>
+      </c>
+      <c r="E3">
+        <v>1.9611641</v>
+      </c>
+      <c r="F3">
+        <v>6.6500199999999995E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.3930377</v>
+      </c>
+      <c r="H3">
+        <v>4.9914260000000002E-2</v>
+      </c>
+      <c r="I3">
+        <v>1.0804151</v>
+      </c>
       <c r="J3" s="1">
-        <v>2.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>2.13</v>
+      </c>
+      <c r="K3">
+        <f>1/((H3+I3)*J3)</f>
+        <v>0.41535112215002312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
         <v>17</v>
       </c>
+      <c r="D4">
+        <v>0.10365949000000001</v>
+      </c>
+      <c r="E4">
+        <v>1.5478578999999999</v>
+      </c>
+      <c r="F4">
+        <v>6.2288925000000002E-2</v>
+      </c>
+      <c r="G4">
+        <v>1.2127775000000001</v>
+      </c>
+      <c r="H4">
+        <v>4.7591759999999997E-2</v>
+      </c>
+      <c r="I4">
+        <v>1.1029040000000001</v>
+      </c>
       <c r="J4">
         <v>1.048</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <f t="shared" ref="K4:K8" si="0">1/((H4+I4)*J4)</f>
+        <v>0.82938026062994152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -567,8 +617,12 @@
       <c r="J5">
         <v>2.2389999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0.44802010252729335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" t="s">
@@ -595,8 +649,12 @@
       <c r="J6">
         <v>1.1870000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0.48551316377908121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -627,8 +685,12 @@
       <c r="J7">
         <v>2.4060000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <f>1/((H7+I7)*J7)</f>
+        <v>0.23706565746095754</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
@@ -655,8 +717,12 @@
       <c r="J8">
         <v>1.2390000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0.46398025092882256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>11</v>
       </c>
@@ -667,7 +733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -690,17 +756,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Added results of performance per categories
On epoch 10
</commit_message>
<xml_diff>
--- a/Structure tables report.xlsx
+++ b/Structure tables report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gines\Desktop\DLVR_3DReconstruction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4B1FB3-2BFE-45F3-992A-9E14E9F4B02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E76C594-34F9-4F5A-847B-18C2312152F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12666EA-FB6F-4139-A86C-FF6F095F9F2F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E12666EA-FB6F-4139-A86C-FF6F095F9F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Net</t>
   </si>
@@ -50,9 +50,6 @@
     <t>10 epochs</t>
   </si>
   <si>
-    <t>Incep variable</t>
-  </si>
-  <si>
     <t>Depth</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>Sweater</t>
   </si>
   <si>
-    <t>Towel</t>
-  </si>
-  <si>
     <t>Paper</t>
   </si>
   <si>
@@ -96,6 +90,21 @@
   </si>
   <si>
     <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Cloth</t>
+  </si>
+  <si>
+    <t>Hoody</t>
+  </si>
+  <si>
+    <t>Tshirt</t>
+  </si>
+  <si>
+    <t>&lt;--------</t>
+  </si>
+  <si>
+    <t>After 10 epochs in this table :)</t>
   </si>
 </sst>
 </file>
@@ -454,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574D92E5-B77D-4ABF-923C-B73F1B547486}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,7 +477,7 @@
     <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
@@ -482,51 +491,51 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B3" s="2">
         <f>231624+268281+268299</f>
         <v>768204</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>0.13387018000000001</v>
@@ -554,11 +563,11 @@
         <v>0.41535112215002312</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>0.10365949000000001</v>
@@ -586,15 +595,15 @@
         <v>0.82938026062994152</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2">
         <v>1989452</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>9.4419390000000006E-2</v>
@@ -622,11 +631,11 @@
         <v>0.44802010252729335</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>9.0334860000000003E-2</v>
@@ -654,15 +663,15 @@
         <v>0.48551316377908121</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2">
         <v>10756132</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>0.117326826</v>
@@ -690,11 +699,11 @@
         <v>0.23706565746095754</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>0.10224973</v>
@@ -722,57 +731,307 @@
         <v>0.46398025092882256</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
       <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
         <v>5</v>
       </c>
-      <c r="G11" t="s">
-        <v>6</v>
-      </c>
       <c r="H11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" t="s">
         <v>5</v>
       </c>
-      <c r="I11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="J11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="K11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2">
+        <f>231624+268281+268299</f>
+        <v>768204</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>3.7727453000000001E-2</v>
+      </c>
+      <c r="E12">
+        <v>1.0407907999999999</v>
+      </c>
+      <c r="F12">
+        <v>8.8872690000000004E-2</v>
+      </c>
+      <c r="G12">
+        <v>1.298073</v>
+      </c>
+      <c r="H12">
+        <v>6.4535910000000002E-2</v>
+      </c>
+      <c r="I12">
+        <v>1.3023244</v>
+      </c>
+      <c r="J12">
+        <v>7.8107949999999995E-2</v>
+      </c>
+      <c r="K12">
+        <v>1.3971530000000001</v>
+      </c>
+      <c r="L12">
+        <v>6.2479510000000002E-2</v>
+      </c>
+      <c r="M12">
+        <v>1.1054889000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>3.6929759999999999E-2</v>
+      </c>
+      <c r="E13">
+        <v>1.0440722</v>
+      </c>
+      <c r="F13">
+        <v>9.3535660000000007E-2</v>
+      </c>
+      <c r="G13">
+        <v>1.3148359999999999</v>
+      </c>
+      <c r="H13">
+        <v>5.7419900000000003E-2</v>
+      </c>
+      <c r="I13">
+        <v>1.3108557000000001</v>
+      </c>
+      <c r="J13">
+        <v>7.0308579999999996E-2</v>
+      </c>
+      <c r="K13">
+        <v>1.4024817000000001</v>
+      </c>
+      <c r="L13">
+        <v>6.0015798000000002E-2</v>
+      </c>
+      <c r="M13">
+        <v>1.0940189</v>
+      </c>
+      <c r="N13" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B14" s="2">
+        <v>1989452</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>3.3315957E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.88682019999999995</v>
+      </c>
+      <c r="F14">
+        <v>7.0560250000000005E-2</v>
+      </c>
+      <c r="G14">
+        <v>1.1872355000000001</v>
+      </c>
+      <c r="H14">
+        <v>4.7023280000000001E-2</v>
+      </c>
+      <c r="I14">
+        <v>1.1152321000000001</v>
+      </c>
+      <c r="J14">
+        <v>5.0319959999999997E-2</v>
+      </c>
+      <c r="K14">
+        <v>1.190321</v>
+      </c>
+      <c r="L14">
+        <v>4.9251344000000002E-2</v>
+      </c>
+      <c r="M14">
+        <v>0.97129509999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>5.1807974E-2</v>
+      </c>
+      <c r="E15">
+        <v>1.5437989000000001</v>
+      </c>
+      <c r="F15">
+        <v>8.4237350000000003E-2</v>
+      </c>
+      <c r="G15">
+        <v>1.9795997000000001</v>
+      </c>
+      <c r="H15">
+        <v>6.3675910000000002E-2</v>
+      </c>
+      <c r="I15">
+        <v>1.8204632000000001</v>
+      </c>
+      <c r="J15">
+        <v>7.6809310000000006E-2</v>
+      </c>
+      <c r="K15">
+        <v>2.0459866999999998</v>
+      </c>
+      <c r="L15">
+        <v>6.038789E-2</v>
+      </c>
+      <c r="M15">
+        <v>1.8239620000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2">
+        <v>10756132</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>6.3842040000000003E-2</v>
+      </c>
+      <c r="E16">
+        <v>1.5262985</v>
+      </c>
+      <c r="F16">
+        <v>0.10952318</v>
+      </c>
+      <c r="G16">
+        <v>1.9895621999999999</v>
+      </c>
+      <c r="H16">
+        <v>9.2206389999999999E-2</v>
+      </c>
+      <c r="I16">
+        <v>1.8147032000000001</v>
+      </c>
+      <c r="J16">
+        <v>9.4131770000000003E-2</v>
+      </c>
+      <c r="K16">
+        <v>2.0846285999999998</v>
+      </c>
+      <c r="L16">
+        <v>8.1547819999999993E-2</v>
+      </c>
+      <c r="M16">
+        <v>1.8472519000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>5.6296843999999999E-2</v>
+      </c>
+      <c r="E17">
+        <v>1.5438864999999999</v>
+      </c>
+      <c r="F17">
+        <v>0.107318565</v>
+      </c>
+      <c r="G17">
+        <v>1.9878129</v>
+      </c>
+      <c r="H17">
+        <v>9.0307854000000007E-2</v>
+      </c>
+      <c r="I17">
+        <v>1.8178124</v>
+      </c>
+      <c r="J17">
+        <v>8.854476E-2</v>
+      </c>
+      <c r="K17">
+        <v>2.0514804999999998</v>
+      </c>
+      <c r="L17">
+        <v>7.9266009999999998E-2</v>
+      </c>
+      <c r="M17">
+        <v>1.8279300000000001</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="15">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>

</xml_diff>